<commit_message>
program to add edges
</commit_message>
<xml_diff>
--- a/edge_cons.xlsx
+++ b/edge_cons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varaunight/Desktop/Tunnel Mapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07149E7D-E616-6446-B42E-C36E90571A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A382BDD-7348-4D4D-9CD8-E25C43E44098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,92 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>SLC</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>RCH</t>
+  </si>
+  <si>
+    <t>DWE</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>QNC</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>PHYS</t>
+  </si>
+  <si>
+    <t>EV1</t>
+  </si>
+  <si>
+    <t>EV2</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>EV3</t>
+  </si>
+  <si>
+    <t>PAS</t>
+  </si>
+  <si>
+    <t>SCH</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,14 +455,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+      <selection activeCell="C16" sqref="A16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>